<commit_message>
retirada da borda da imagem dos gráficos de medicamentos aparecida e jacareí
</commit_message>
<xml_diff>
--- a/Dados/Dados de Medicamentos/Gasto Medicamento Finalizado - Jacareí.xlsx
+++ b/Dados/Dados de Medicamentos/Gasto Medicamento Finalizado - Jacareí.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/120fd542a8b8b6a0/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\API\Dados\Dados de Medicamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0994F1A-B5E6-4E7F-B91C-AF9812716ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05DD2C47-ECB9-4195-A4A4-46D79EBF632B}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
@@ -87,8 +86,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -220,67 +247,6 @@
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Planilha1!$A$2:$A$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2022</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Planilha1!$A$2:$A$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2022</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-984B-4311-974A-D0CE83777D7E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -430,6 +396,85 @@
         <c:overlap val="-27"/>
         <c:axId val="1282906783"/>
         <c:axId val="1282913983"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$A$2:$A$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2021</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2022</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$A$2:$A$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2021</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2022</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-984B-4311-974A-D0CE83777D7E}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="1282906783"/>
@@ -530,6 +575,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -605,6 +651,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -612,7 +659,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1527,19 +1573,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D22A3A-5922-4354-8C71-131A15261AC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1555,7 +1601,7 @@
         <v>9276151.2400000002</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -1563,7 +1609,7 @@
         <v>14695626.92</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -1571,7 +1617,7 @@
         <v>13989926.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2022</v>
       </c>

</xml_diff>